<commit_message>
Letzter Stand 1603(Transfer auf Laptop wegen Corona)
</commit_message>
<xml_diff>
--- a/Protocol/COM_Protocol_V0_0_6.xlsx
+++ b/Protocol/COM_Protocol_V0_0_6.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="131">
   <si>
     <t>Befehl</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>1000..20000</t>
-  </si>
-  <si>
-    <t>(Mess-Spannung in  mV)</t>
   </si>
   <si>
     <t>SHC[N]M= xmV</t>
@@ -418,6 +415,33 @@
   </si>
   <si>
     <t>SWG[N]F = xW/O-Unit</t>
+  </si>
+  <si>
+    <t>SIN[N]M</t>
+  </si>
+  <si>
+    <t>Initialisierung für „MOSFET-Source“ Karte</t>
+  </si>
+  <si>
+    <t>(Mess-Spannung in  0,1 V)</t>
+  </si>
+  <si>
+    <t>GHC[N]M</t>
+  </si>
+  <si>
+    <t>GMC[N]M</t>
+  </si>
+  <si>
+    <t>GMV[N]M</t>
+  </si>
+  <si>
+    <t>GHC[N]M= xmA</t>
+  </si>
+  <si>
+    <t>GMC[N]M= x.xmA</t>
+  </si>
+  <si>
+    <t>GHC[N]M= xmV</t>
   </si>
 </sst>
 </file>
@@ -653,6 +677,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -667,9 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J42"/>
+  <dimension ref="B2:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,18 +991,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="H2" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1011,14 +1035,14 @@
       <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3"/>
       <c r="H5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="19"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1038,7 +1062,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>9</v>
@@ -1051,14 +1075,14 @@
       <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="7"/>
       <c r="H7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1078,10 +1102,10 @@
         <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>10</v>
@@ -1104,7 +1128,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6" t="s">
@@ -1128,7 +1152,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="6" t="s">
@@ -1152,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
@@ -1163,14 +1187,14 @@
       <c r="B12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="7"/>
       <c r="H12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="19"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1190,7 +1214,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>28</v>
@@ -1216,7 +1240,7 @@
         <v>10</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>31</v>
@@ -1242,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>35</v>
@@ -1268,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>38</v>
@@ -1285,7 +1309,7 @@
         <v>40</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>41</v>
@@ -1294,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>41</v>
@@ -1307,14 +1331,14 @@
       <c r="B18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
       <c r="H18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="19"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1325,17 +1349,17 @@
         <v>44</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>45</v>
@@ -1348,14 +1372,14 @@
       <c r="B20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="8"/>
       <c r="H20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="19"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1372,10 +1396,10 @@
         <v>47</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6" t="s">
@@ -1399,7 +1423,7 @@
         <v>10</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>53</v>
@@ -1425,7 +1449,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>57</v>
@@ -1438,386 +1462,408 @@
       <c r="B24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="9"/>
       <c r="H24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="10"/>
+        <v>122</v>
+      </c>
+      <c r="F25" s="12"/>
       <c r="H25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="10"/>
+        <v>98</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F26" s="10"/>
       <c r="H26" s="4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F27" s="10"/>
       <c r="H27" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="C28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="H28" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="9"/>
+      <c r="H29" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" s="20"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="9"/>
+      <c r="H32" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="9"/>
-      <c r="H28" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="9"/>
-      <c r="H31" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="H32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J32" s="10"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="9"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="F33" s="10"/>
       <c r="H33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="22"/>
-      <c r="H34" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="22"/>
+      <c r="D34" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="10"/>
+      <c r="H34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="H35" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J35" s="10"/>
+      <c r="B35" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="23"/>
+      <c r="H35" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="22"/>
+      <c r="J35" s="23"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F36" s="10"/>
       <c r="H36" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J36" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="F40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I39" s="5" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="9"/>
+      <c r="H41" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="18" t="s">
+      <c r="I41" s="20"/>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="9"/>
-      <c r="H40" s="18" t="s">
+      <c r="C42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I40" s="19"/>
-      <c r="J40" s="9"/>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="I42" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H29:I29"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
@@ -1826,13 +1872,13 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSFET Source und LED Source richtig
</commit_message>
<xml_diff>
--- a/Protocol/COM_Protocol_V0_0_6.xlsx
+++ b/Protocol/COM_Protocol_V0_0_6.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmidm\Desktop\MC_RthTEC_Programm\MC_RthTEC_V_0_GIT\Protocol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmidm\Desktop\MC_ATIM\Protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5281DD29-A4AF-4ADD-8941-631DAAFCCDAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="136">
   <si>
     <t>Befehl</t>
   </si>
@@ -222,9 +223,6 @@
   </si>
   <si>
     <t>1000..20000</t>
-  </si>
-  <si>
-    <t>SHC[N]M= xmV</t>
   </si>
   <si>
     <t>4.3 AD-Unit                         (A)</t>
@@ -423,9 +421,6 @@
     <t>Initialisierung für „MOSFET-Source“ Karte</t>
   </si>
   <si>
-    <t>(Mess-Spannung in  0,1 V)</t>
-  </si>
-  <si>
     <t>GHC[N]M</t>
   </si>
   <si>
@@ -441,13 +436,34 @@
     <t>GMC[N]M= x.xmA</t>
   </si>
   <si>
-    <t>GHC[N]M= xmV</t>
+    <t>SHC[N]M= x.xxV</t>
+  </si>
+  <si>
+    <t>GHC[N]M= x.xxV</t>
+  </si>
+  <si>
+    <t>GHM[N]M</t>
+  </si>
+  <si>
+    <t>GMM[N]M</t>
+  </si>
+  <si>
+    <t>GHM[N]M= x.xxxV</t>
+  </si>
+  <si>
+    <t>(Eingestellte Mess-Spannung in  0,1 V)</t>
+  </si>
+  <si>
+    <t>(Gemessene Mess-Spannung in  V)</t>
+  </si>
+  <si>
+    <t>(Gemessene (measured) Heiz-Spannung in  V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,7 +549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -617,11 +633,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -677,23 +733,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,11 +1048,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,18 +1065,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="H2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="H2" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1035,14 +1109,14 @@
       <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="3"/>
       <c r="H5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1062,7 +1136,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>9</v>
@@ -1075,14 +1149,14 @@
       <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="7"/>
       <c r="H7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1102,10 +1176,10 @@
         <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>10</v>
@@ -1128,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6" t="s">
@@ -1152,7 +1226,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="6" t="s">
@@ -1176,7 +1250,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
@@ -1187,14 +1261,14 @@
       <c r="B12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="7"/>
       <c r="H12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="19"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1214,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>28</v>
@@ -1240,7 +1314,7 @@
         <v>10</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>31</v>
@@ -1266,7 +1340,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>35</v>
@@ -1292,7 +1366,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>38</v>
@@ -1309,7 +1383,7 @@
         <v>40</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>41</v>
@@ -1318,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>41</v>
@@ -1331,14 +1405,14 @@
       <c r="B18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="8"/>
       <c r="H18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="20"/>
+      <c r="I18" s="19"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1349,17 +1423,17 @@
         <v>44</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>45</v>
@@ -1372,14 +1446,14 @@
       <c r="B20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="8"/>
       <c r="H20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="20"/>
+      <c r="I20" s="19"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1396,10 +1470,10 @@
         <v>47</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6" t="s">
@@ -1423,7 +1497,7 @@
         <v>10</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>53</v>
@@ -1449,7 +1523,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>57</v>
@@ -1462,32 +1536,34 @@
       <c r="B24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="9"/>
       <c r="H24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="19"/>
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" s="12"/>
+        <v>121</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H25" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="6" t="s">
@@ -1507,14 +1583,18 @@
       <c r="E26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="12" t="s">
+        <v>107</v>
+      </c>
       <c r="H26" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="J26" s="10"/>
+        <v>126</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
@@ -1529,341 +1609,393 @@
       <c r="E27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H27" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I27" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="J28" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="30"/>
+      <c r="F29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="9"/>
+      <c r="H31" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I31" s="19"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="9"/>
+      <c r="H34" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="H28" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J28" s="10"/>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="9"/>
-      <c r="H29" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="I34" s="19"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="9"/>
-      <c r="H32" s="18" t="s">
+      <c r="E35" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="H35" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="I35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" s="10"/>
-      <c r="H33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="10"/>
-      <c r="H34" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I34" s="5"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="23"/>
-      <c r="H35" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" s="22"/>
-      <c r="J35" s="23"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E36" s="5"/>
       <c r="F36" s="10"/>
       <c r="H36" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I36" s="5"/>
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J37" s="6"/>
+      <c r="B37" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22"/>
+      <c r="H37" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="21"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F38" s="10"/>
       <c r="H38" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J38" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="9"/>
-      <c r="H41" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="9"/>
+      <c r="B41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J41" s="6"/>
     </row>
     <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="9"/>
+      <c r="H43" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I43" s="19"/>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="F44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B31:E31"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
@@ -1872,13 +2004,13 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H31:I31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
All Slot-Cards implemented and working
</commit_message>
<xml_diff>
--- a/Protocol/COM_Protocol_V0_0_6.xlsx
+++ b/Protocol/COM_Protocol_V0_0_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmidm\Desktop\MC_ATIM\Protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5281DD29-A4AF-4ADD-8941-631DAAFCCDAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C82450-7A72-40D8-AA7D-6DF923EC9743}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,162 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>schmidm</author>
+  </authors>
+  <commentList>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{DF59B4CC-C4BF-4837-B889-6839AE1281D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>schmidm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wird automatisch ausgeführt wenn Karten Typ geändert wird</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{C15CFBD2-3523-490B-BA14-EA830C480183}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>schmidm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wird automatisch ausgeführt wenn Karten Typ geändert wird</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{492224F5-DE2E-47D2-BA41-8F87175160FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>schmidm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wird automatisch ausgeführt wenn Karten Typ geändert wird</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{2375081B-5A28-4FE0-842E-342DF59C00F3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>schmidm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wird automatisch ausgeführt wenn Karten Typ geändert wird</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{3513DDD4-F8CF-446A-BCBE-B6D0618D1F29}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>schmidm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wird automatisch ausgeführt wenn Karten Typ geändert wird</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="0" shapeId="0" xr:uid="{5F634D68-2CF6-491D-B2C3-AA6544E6C89A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>schmidm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wird automatisch ausgeführt wenn Karten Typ geändert wird</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="169">
   <si>
     <t>Befehl</t>
   </si>
@@ -174,9 +328,6 @@
     <t>keine</t>
   </si>
   <si>
-    <t>Initialisierung für „LED-Source“ Karte</t>
-  </si>
-  <si>
     <t>SHC[N]L</t>
   </si>
   <si>
@@ -237,27 +388,12 @@
     <t>(Offset in mV)</t>
   </si>
   <si>
-    <t>SWO = xmV</t>
-  </si>
-  <si>
-    <t>SWW[N][X]</t>
-  </si>
-  <si>
-    <t>50 | 100| 200</t>
-  </si>
-  <si>
-    <t>(Auflösung in mV)</t>
-  </si>
-  <si>
     <t>4.4 MOSFET Break-Down    (B)</t>
   </si>
   <si>
     <t>SIN[N]B</t>
   </si>
   <si>
-    <t>Initialisierung für „Break Down-Card“</t>
-  </si>
-  <si>
     <t>SRB[N]B</t>
   </si>
   <si>
@@ -300,25 +436,7 @@
     <t>SST[N]T</t>
   </si>
   <si>
-    <t>Set Slot Tester</t>
-  </si>
-  <si>
     <t>SST Slot-Test: [N]</t>
-  </si>
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Soll später über SCT ausgefürht werden</t>
-    </r>
   </si>
   <si>
     <t>SET</t>
@@ -382,9 +500,6 @@
 Beginnend mit Slot 1 (MSB)</t>
   </si>
   <si>
-    <t>4.3 AD-Unit (THI)              (A)</t>
-  </si>
-  <si>
     <t>4.3 FrontEnd Heller         (H)</t>
   </si>
   <si>
@@ -418,9 +533,6 @@
     <t>SIN[N]M</t>
   </si>
   <si>
-    <t>Initialisierung für „MOSFET-Source“ Karte</t>
-  </si>
-  <si>
     <t>GHC[N]M</t>
   </si>
   <si>
@@ -458,13 +570,148 @@
   </si>
   <si>
     <t>(Gemessene (measured) Heiz-Spannung in  V)</t>
+  </si>
+  <si>
+    <t>4.3.1 FrontEnd Heller         (H)</t>
+  </si>
+  <si>
+    <t>4.3.2 Amplifier-Unit (THI)              (A)</t>
+  </si>
+  <si>
+    <t>4.99 Slot-Tester                        (T)</t>
+  </si>
+  <si>
+    <t>SIN[N]F</t>
+  </si>
+  <si>
+    <t>SIN[N]A</t>
+  </si>
+  <si>
+    <t>SIN[N]T</t>
+  </si>
+  <si>
+    <t>(Window Gain (EinheitenLos) [geht nur 2])</t>
+  </si>
+  <si>
+    <t>SWG[N]A</t>
+  </si>
+  <si>
+    <t>GWO[N]A</t>
+  </si>
+  <si>
+    <t>GWG[N]A</t>
+  </si>
+  <si>
+    <t>SWG[N]A = 2 W/O-Unit</t>
+  </si>
+  <si>
+    <t>SWO[N]A = xmV</t>
+  </si>
+  <si>
+    <t>GWO[N]A = xmV</t>
+  </si>
+  <si>
+    <t>GWG[N]A = 2 W/O-Unit</t>
+  </si>
+  <si>
+    <t>SRF[N]F</t>
+  </si>
+  <si>
+    <t>Reset FlipFlops</t>
+  </si>
+  <si>
+    <t>GSI[N]F</t>
+  </si>
+  <si>
+    <t>Get IO-Expander Info</t>
+  </si>
+  <si>
+    <t>GVF[N]F</t>
+  </si>
+  <si>
+    <t>Get Voltage fullrange ADC</t>
+  </si>
+  <si>
+    <t>GWG[N]F = xW/O-Unit</t>
+  </si>
+  <si>
+    <t>GWO[N]F = xmV</t>
+  </si>
+  <si>
+    <t>GVF[N]F =x mV</t>
+  </si>
+  <si>
+    <t>0 … 9</t>
+  </si>
+  <si>
+    <t>Set Displayl Number</t>
+  </si>
+  <si>
+    <t>SDN[N]T</t>
+  </si>
+  <si>
+    <t>SDN[N]T = x</t>
+  </si>
+  <si>
+    <t>GDN[N]T</t>
+  </si>
+  <si>
+    <t>GDN[N]T = x</t>
+  </si>
+  <si>
+    <t>Initialisierung für „Slot-Tester“
+Changes slot card typ only for this slot + default setting</t>
+  </si>
+  <si>
+    <t>GHC[N]L= xmA</t>
+  </si>
+  <si>
+    <t>GMC[N]L= x.xmA</t>
+  </si>
+  <si>
+    <t>GCT = LMA00000</t>
+  </si>
+  <si>
+    <t>GRB[N]B=1</t>
+  </si>
+  <si>
+    <t>GRL[N]B=1</t>
+  </si>
+  <si>
+    <t>GRC[N]B=1</t>
+  </si>
+  <si>
+    <t>GRD[N]B=1</t>
+  </si>
+  <si>
+    <t>Set Slot Run (Runs all LEDs and SPI) Answer when finished</t>
+  </si>
+  <si>
+    <t>Initialisierung für „Break Down-Card“
+Changes slot card typ only for this slot + default setting</t>
+  </si>
+  <si>
+    <t>Initialisierung für „Amplifier THI“
+Changes slot card typ only for this slot + default setting</t>
+  </si>
+  <si>
+    <t>Initialisierung für „FrontEnd Heller“
+Changes slot card typ only for this slot + default setting</t>
+  </si>
+  <si>
+    <t>Initialisierung für „MOSFET-Source“ Karte
+Changes slot card typ only for this slot + default setting</t>
+  </si>
+  <si>
+    <t>Initialisierung für „LED-Source“ Karte
+Changes slot card typ only for this slot + default setting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +780,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -677,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -730,9 +990,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -745,29 +1017,20 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,35 +1311,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="9" max="9" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="H2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="H2" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1106,17 +1369,17 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="19"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="19"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1136,7 +1399,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>9</v>
@@ -1146,17 +1409,17 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="7"/>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1176,10 +1439,10 @@
         <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>10</v>
@@ -1202,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6" t="s">
@@ -1226,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="6" t="s">
@@ -1250,7 +1513,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
@@ -1258,17 +1521,17 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="7"/>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="19"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1288,7 +1551,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>28</v>
@@ -1314,7 +1577,7 @@
         <v>10</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>31</v>
@@ -1340,7 +1603,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>35</v>
@@ -1366,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>38</v>
@@ -1383,7 +1646,7 @@
         <v>40</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>41</v>
@@ -1392,7 +1655,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>41</v>
@@ -1402,17 +1665,17 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="8"/>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="19"/>
+      <c r="I18" s="23"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1423,40 +1686,40 @@
         <v>44</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="13" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="8"/>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="19"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1464,16 +1727,16 @@
         <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>168</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6" t="s">
@@ -1482,25 +1745,25 @@
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>53</v>
+        <v>156</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>10</v>
@@ -1508,62 +1771,62 @@
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="5" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="9"/>
+      <c r="H24" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="9"/>
-      <c r="H24" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="23"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="6" t="s">
@@ -1572,121 +1835,121 @@
     </row>
     <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="F26" s="12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="4" t="s">
+      <c r="C28" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="30"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>10</v>
@@ -1694,308 +1957,466 @@
     </row>
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="27" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
       <c r="F31" s="9"/>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" s="23"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="9"/>
-      <c r="H34" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="9"/>
+      <c r="F34" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="10"/>
+        <v>141</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="12"/>
       <c r="H35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J35" s="10"/>
+        <v>89</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>72</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="F36" s="10"/>
+      <c r="F36" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H36" s="4" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="I36" s="5"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
-      <c r="H37" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="22"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="10"/>
-      <c r="H38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J38" s="10"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="9"/>
+      <c r="H38" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="23"/>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>79</v>
+        <v>165</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J39" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F40" s="10"/>
       <c r="H40" s="4" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J40" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>7</v>
+        <v>133</v>
+      </c>
+      <c r="C41" s="31">
+        <v>2</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F41" s="10"/>
       <c r="H41" s="4" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J41" s="6"/>
+        <v>139</v>
+      </c>
+      <c r="J41" s="10"/>
     </row>
     <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
+      <c r="B42" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="26"/>
+      <c r="H42" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" s="25"/>
+      <c r="J42" s="26"/>
+    </row>
+    <row r="43" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="9"/>
-      <c r="H43" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="I43" s="19"/>
-      <c r="J43" s="9"/>
+      <c r="I43" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="H44" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="H45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="H46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="H47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="9"/>
+      <c r="H48" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I48" s="23"/>
+      <c r="J48" s="9"/>
+    </row>
+    <row r="49" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="D49" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I49" s="5"/>
+      <c r="J49" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
@@ -2004,15 +2425,16 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Firmware/Softwere/Hardware Version + Manufacturing Date
</commit_message>
<xml_diff>
--- a/Protocol/COM_Protocol_V0_0_6.xlsx
+++ b/Protocol/COM_Protocol_V0_0_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmidm\Desktop\MC_ATIM\Protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C82450-7A72-40D8-AA7D-6DF923EC9743}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977E9F77-76D4-476C-8512-5F9F5A094C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>schmidm</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{DF59B4CC-C4BF-4837-B889-6839AE1281D9}">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{DF59B4CC-C4BF-4837-B889-6839AE1281D9}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{C15CFBD2-3523-490B-BA14-EA830C480183}">
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{C15CFBD2-3523-490B-BA14-EA830C480183}">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{492224F5-DE2E-47D2-BA41-8F87175160FF}">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{492224F5-DE2E-47D2-BA41-8F87175160FF}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{2375081B-5A28-4FE0-842E-342DF59C00F3}">
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{2375081B-5A28-4FE0-842E-342DF59C00F3}">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{3513DDD4-F8CF-446A-BCBE-B6D0618D1F29}">
+    <comment ref="B50" authorId="0" shapeId="0" xr:uid="{3513DDD4-F8CF-446A-BCBE-B6D0618D1F29}">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0" shapeId="0" xr:uid="{5F634D68-2CF6-491D-B2C3-AA6544E6C89A}">
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{5F634D68-2CF6-491D-B2C3-AA6544E6C89A}">
       <text>
         <r>
           <rPr>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="191">
   <si>
     <t>Befehl</t>
   </si>
@@ -705,6 +705,72 @@
   <si>
     <t>Initialisierung für „LED-Source“ Karte
 Changes slot card typ only for this slot + default setting</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>reboot</t>
+  </si>
+  <si>
+    <t>Reset the µC</t>
+  </si>
+  <si>
+    <t>0.1 RST</t>
+  </si>
+  <si>
+    <t>0.2 Info</t>
+  </si>
+  <si>
+    <t>GID</t>
+  </si>
+  <si>
+    <t>GSV</t>
+  </si>
+  <si>
+    <t>GHW</t>
+  </si>
+  <si>
+    <t>GMD</t>
+  </si>
+  <si>
+    <t>Software Version</t>
+  </si>
+  <si>
+    <t>Identification string</t>
+  </si>
+  <si>
+    <t>0.1 Reset</t>
+  </si>
+  <si>
+    <t>GID=RthTEC mC Unit</t>
+  </si>
+  <si>
+    <t>GSV=x.x.x.x</t>
+  </si>
+  <si>
+    <t>GHV=x.x</t>
+  </si>
+  <si>
+    <t>SHW</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>Hardware Version (setting only one time)</t>
+  </si>
+  <si>
+    <t>Manufacturing Date (setting only one time)</t>
+  </si>
+  <si>
+    <t>GMD=CW[WW]-[JJJJ]</t>
+  </si>
+  <si>
+    <t>[WW]-[JJJJ]</t>
+  </si>
+  <si>
+    <t>Vx.x</t>
   </si>
 </sst>
 </file>
@@ -999,24 +1065,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1025,12 +1097,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1312,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J52"/>
+  <dimension ref="B2:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,18 +1394,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="H2" s="30" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="H2" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1369,80 +1435,72 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="B5" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="23"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="21" t="s">
-        <v>5</v>
+      <c r="H5" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>9</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="I6" s="5"/>
       <c r="J6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="B7" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="21" t="s">
-        <v>11</v>
+      <c r="F7" s="3"/>
+      <c r="H7" s="22" t="s">
+        <v>173</v>
       </c>
       <c r="I7" s="23"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>10</v>
@@ -1450,163 +1508,149 @@
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="J9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>183</v>
+      </c>
       <c r="J10" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>185</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="7"/>
-      <c r="H12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>10</v>
-      </c>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>10</v>
@@ -1614,156 +1658,163 @@
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>101</v>
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="I17" s="5"/>
       <c r="J17" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="8"/>
-      <c r="H18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="8"/>
-      <c r="H20" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="23"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>168</v>
+        <v>30</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>99</v>
+        <v>31</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J21" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>10</v>
@@ -1771,249 +1822,246 @@
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="8"/>
+      <c r="H25" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="23"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="8"/>
+      <c r="H27" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="23"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="4" t="s">
+      <c r="F30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="21" t="s">
+      <c r="J30" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="9"/>
-      <c r="H24" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="27" t="s">
-        <v>126</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
-      <c r="E31" s="29"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="9"/>
-      <c r="H31" s="21" t="s">
-        <v>102</v>
+      <c r="H31" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="I31" s="23"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>99</v>
+        <v>167</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>89</v>
       </c>
       <c r="I32" s="5"/>
-      <c r="J32" s="12" t="s">
-        <v>99</v>
+      <c r="J32" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>99</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>99</v>
@@ -2021,417 +2069,581 @@
     </row>
     <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>99</v>
+        <v>62</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>99</v>
+        <v>117</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F35" s="12"/>
+      <c r="B35" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="H35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="20"/>
+      <c r="F36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I36" s="5"/>
-      <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="6" t="s">
+      <c r="C37" s="20"/>
+      <c r="D37" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="20"/>
+      <c r="F37" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>148</v>
+        <v>121</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="23"/>
+      <c r="B38" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="9"/>
-      <c r="H38" s="21" t="s">
-        <v>65</v>
+      <c r="H38" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="I38" s="23"/>
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>10</v>
+        <v>129</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>89</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="J39" s="6" t="s">
-        <v>10</v>
+      <c r="J39" s="12" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F40" s="10"/>
+        <v>110</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="H40" s="4" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="J40" s="10"/>
+        <v>147</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" s="31">
-        <v>2</v>
+        <v>107</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="10"/>
+        <v>111</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="H41" s="4" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="J41" s="10"/>
+        <v>146</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="26"/>
-      <c r="H42" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="26"/>
-    </row>
-    <row r="43" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="H42" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="J42" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="E43" s="5"/>
       <c r="F43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H43" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="6"/>
+        <v>145</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H44" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J44" s="6"/>
+        <v>144</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="H45" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="9"/>
+      <c r="H45" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="23"/>
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="6"/>
+        <v>165</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H46" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="J46" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="J46" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="H47" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="J47" s="10"/>
+    </row>
+    <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="21">
+        <v>2</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="H48" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="26"/>
+      <c r="H49" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I49" s="25"/>
+      <c r="J49" s="26"/>
+    </row>
+    <row r="50" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="H51" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="H52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="H53" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="H47" s="4" t="s">
+      <c r="F54" s="6"/>
+      <c r="H54" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="I54" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="21" t="s">
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="9"/>
-      <c r="H48" s="21" t="s">
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="9"/>
+      <c r="H55" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="I48" s="23"/>
-      <c r="J48" s="9"/>
-    </row>
-    <row r="49" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
+      <c r="I55" s="23"/>
+      <c r="J55" s="9"/>
+    </row>
+    <row r="56" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="4" t="s">
+      <c r="F56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I49" s="5"/>
-      <c r="J49" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="4" t="s">
+      <c r="I56" s="5"/>
+      <c r="J56" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="4" t="s">
+      <c r="F57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="I57" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="J50" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="4" t="s">
+      <c r="J57" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E58" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="4" t="s">
+      <c r="F58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="H24:I24"/>
+  <mergeCells count="26">
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H27:I27"/>
     <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>